<commit_message>
Auto-committed on 2022/06/16 週四 17:13:10.54
</commit_message>
<xml_diff>
--- a/Program/Other/LM029_底稿_放款餘額明細表.xlsx
+++ b/Program/Other/LM029_底稿_放款餘額明細表.xlsx
@@ -5,34 +5,25 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SKL\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7580"/>
   </bookViews>
   <sheets>
     <sheet name="la$w30p" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'la$w30p'!$A$1:$U$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'la$w30p'!$A$5:$U$5</definedName>
     <definedName name="_xlnm.Database">'la$w30p'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>戶號</t>
   </si>
@@ -80,6 +71,52 @@
   </si>
   <si>
     <t>撥款金額</t>
+  </si>
+  <si>
+    <t>逾期數</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>機密等級：密</t>
+  </si>
+  <si>
+    <t>程式ID：</t>
+  </si>
+  <si>
+    <t>新光人壽保險股份有限公司</t>
+  </si>
+  <si>
+    <t>日　　期：</t>
+  </si>
+  <si>
+    <t>報　表：</t>
+  </si>
+  <si>
+    <t>時　　間：</t>
+  </si>
+  <si>
+    <t>擔保品代號1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>擔保品代號2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>擔保品編號</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LM029</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>L9803</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>放款餘額明細表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -93,7 +130,7 @@
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -267,6 +304,26 @@
       <family val="1"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -461,7 +518,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -576,8 +633,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -719,8 +791,9 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -763,8 +836,32 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="23" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="10" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="48">
     <cellStyle name="20% - 輔色1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - 輔色2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - 輔色3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -785,6 +882,7 @@
     <cellStyle name="60% - 輔色6" xfId="18" builtinId="52" customBuiltin="1"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="一般 2" xfId="19"/>
+    <cellStyle name="一般 3" xfId="47"/>
     <cellStyle name="一般 3 2" xfId="20"/>
     <cellStyle name="千分位" xfId="21" builtinId="3"/>
     <cellStyle name="千分位 2" xfId="22"/>
@@ -1113,13 +1211,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -1136,65 +1234,197 @@
     <col min="13" max="14" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="20.81640625" style="2" customWidth="1"/>
     <col min="18" max="18" width="12.453125" style="1" customWidth="1"/>
+    <col min="19" max="20" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="10" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="U1" s="14"/>
+    </row>
+    <row r="2" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="U2" s="14"/>
+    </row>
+    <row r="3" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="16"/>
+      <c r="T3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="14"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+      <c r="P4" s="16"/>
+      <c r="Q4" s="16"/>
+      <c r="R4" s="16"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+    </row>
+    <row r="5" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="P5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="12">
-        <f>SUBTOTAL(9,Q2:Q1048576)</f>
+      <c r="Q5" s="12">
+        <f>SUBTOTAL(9,Q6:Q1048576)</f>
         <v>0</v>
       </c>
-      <c r="R1" s="13"/>
+      <c r="R5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="U5" s="10" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U1"/>
+  <autoFilter ref="A5:U5"/>
+  <mergeCells count="7">
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="T4:U4"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="T2:U2"/>
+    <mergeCell ref="C2:S2"/>
+    <mergeCell ref="C3:S3"/>
+    <mergeCell ref="C4:S4"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Auto-committed on 2022/06/17 週五 17:40:09.87
</commit_message>
<xml_diff>
--- a/Program/Other/LM029_底稿_放款餘額明細表.xlsx
+++ b/Program/Other/LM029_底稿_放款餘額明細表.xlsx
@@ -325,7 +325,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -503,18 +503,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -793,7 +781,7 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -802,62 +790,56 @@
     </xf>
     <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="33" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="2" fillId="34" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="3" fillId="33" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="20" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="23" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="47" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="10" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="23" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="23" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="10" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1217,7 +1199,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N25" sqref="N25"/>
+      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -1228,7 +1210,7 @@
     <col min="6" max="6" width="33.36328125" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="15.6328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.90625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.90625" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="18.08984375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
@@ -1239,178 +1221,178 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="14" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="14"/>
+      <c r="U1" s="11"/>
     </row>
     <row r="2" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="14" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="14"/>
+      <c r="U2" s="11"/>
     </row>
     <row r="3" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="16"/>
-      <c r="N3" s="16"/>
-      <c r="O3" s="16"/>
-      <c r="P3" s="16"/>
-      <c r="Q3" s="16"/>
-      <c r="R3" s="16"/>
-      <c r="S3" s="16"/>
-      <c r="T3" s="14" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="14"/>
+      <c r="U3" s="11"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16"/>
-      <c r="S4" s="16"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="11"/>
     </row>
-    <row r="5" spans="1:21" s="10" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="M5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="8" t="s">
+      <c r="O5" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="11" t="s">
+      <c r="P5" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="Q5" s="12">
+      <c r="Q5" s="4">
         <f>SUBTOTAL(9,Q6:Q1048576)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="13" t="s">
+      <c r="R5" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="S5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="T5" s="10" t="s">
+      <c r="T5" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="U5" s="10" t="s">
+      <c r="U5" s="19" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto-committed on 2022/08/18 週四 11:36:18.60
</commit_message>
<xml_diff>
--- a/Program/Other/LM029_底稿_放款餘額明細表.xlsx
+++ b/Program/Other/LM029_底稿_放款餘額明細表.xlsx
@@ -5,25 +5,31 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\weblogic\itxDoc\itxWrite\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7580"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6040" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="la$w30p" sheetId="1" r:id="rId1"/>
+    <sheet name="Deliquency" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'la$w30p'!$A$5:$U$5</definedName>
+    <definedName name="_xlnm.Database" localSheetId="1">#REF!</definedName>
     <definedName name="_xlnm.Database">'la$w30p'!#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Deliquency!#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>戶號</t>
   </si>
@@ -74,7 +80,7 @@
   </si>
   <si>
     <t>逾期數</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>機密等級：密</t>
@@ -96,46 +102,84 @@
   </si>
   <si>
     <t>擔保品代號1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>擔保品代號2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>擔保品編號</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>LM029</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>L9803</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>放款餘額明細表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>人壽放款逾1~2期金額佔放款總額比統計</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>項目</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>逾1-2期金額</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>放款總餘額</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>逾1~2期佔總額比</t>
+    <phoneticPr fontId="28" type="noConversion"/>
+  </si>
+  <si>
+    <t>逾放總額</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>放款逾放比</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0.0000"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="yyyy/mm/dd"/>
+    <numFmt numFmtId="181" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    <numFmt numFmtId="192" formatCode="#,##0;[Red]#,##0"/>
   </numFmts>
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="新細明體"/>
       <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
@@ -324,6 +368,88 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="1"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color indexed="22"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color indexed="8"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -506,7 +632,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -636,177 +762,195 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="20" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="21" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="23" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="47" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="47" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="10" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="10" xfId="21" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -815,35 +959,75 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="23" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="23" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="31" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="192" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="192" fontId="35" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="192" fontId="36" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="35" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="51">
+    <cellStyle name="%" xfId="48"/>
     <cellStyle name="20% - 輔色1" xfId="1" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - 輔色2" xfId="2" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - 輔色3" xfId="3" builtinId="38" customBuiltin="1"/>
@@ -872,6 +1056,8 @@
     <cellStyle name="中等" xfId="24" builtinId="28" customBuiltin="1"/>
     <cellStyle name="合計" xfId="25" builtinId="25" customBuiltin="1"/>
     <cellStyle name="好" xfId="26" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="百分比 2" xfId="49"/>
+    <cellStyle name="百分比 2 2" xfId="50"/>
     <cellStyle name="計算方式" xfId="27" builtinId="22" customBuiltin="1"/>
     <cellStyle name="連結的儲存格" xfId="28" builtinId="24" customBuiltin="1"/>
     <cellStyle name="備註" xfId="29" builtinId="10" customBuiltin="1"/>
@@ -904,6 +1090,19 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Deliquency "/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1195,7 +1394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1240,10 +1439,10 @@
       <c r="Q1" s="8"/>
       <c r="R1" s="9"/>
       <c r="S1" s="10"/>
-      <c r="T1" s="11" t="s">
+      <c r="T1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="11"/>
+      <c r="U1" s="18"/>
     </row>
     <row r="2" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
@@ -1252,29 +1451,29 @@
       <c r="B2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="11" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="11"/>
+      <c r="U2" s="18"/>
     </row>
     <row r="3" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
@@ -1283,116 +1482,116 @@
       <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
-      <c r="T3" s="11" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="11"/>
+      <c r="U3" s="18"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.4">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-    </row>
-    <row r="5" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="13" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19"/>
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="18"/>
+    </row>
+    <row r="5" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="M5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="O5" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="P5" s="18" t="s">
+      <c r="P5" s="16" t="s">
         <v>15</v>
       </c>
       <c r="Q5" s="4">
         <f>SUBTOTAL(9,Q6:Q1048576)</f>
         <v>0</v>
       </c>
-      <c r="R5" s="16" t="s">
+      <c r="R5" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="S5" s="19" t="s">
+      <c r="S5" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="T5" s="19" t="s">
+      <c r="T5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="U5" s="19" t="s">
+      <c r="U5" s="17" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1407,8 +1606,208 @@
     <mergeCell ref="C3:S3"/>
     <mergeCell ref="C4:S4"/>
   </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:BC27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A13" sqref="A13:XFD15"/>
+      <selection pane="topRight" activeCell="A13" sqref="A13:XFD15"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD15"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="27.1796875" style="27" customWidth="1"/>
+    <col min="2" max="2" width="12" style="22" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="22"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="24" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="29" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="29" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="30"/>
+    </row>
+    <row r="5" spans="1:5" s="32" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="29" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="32" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.4">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="B9" s="26"/>
+    </row>
+    <row r="10" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="27"/>
+      <c r="B10" s="22"/>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+    </row>
+    <row r="11" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="27"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+    </row>
+    <row r="12" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="27"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+    </row>
+    <row r="13" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="27"/>
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+    </row>
+    <row r="14" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="27"/>
+      <c r="B14" s="22"/>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+    </row>
+    <row r="15" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="27"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+    </row>
+    <row r="16" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="27"/>
+      <c r="B16" s="22"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+    </row>
+    <row r="17" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="27"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+    </row>
+    <row r="18" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="27"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+    </row>
+    <row r="19" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="27"/>
+      <c r="B19" s="22"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+    </row>
+    <row r="20" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="27"/>
+      <c r="B20" s="22"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+    </row>
+    <row r="21" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="27"/>
+      <c r="B21" s="22"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="22"/>
+    </row>
+    <row r="22" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="27"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+    </row>
+    <row r="23" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="27"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+    </row>
+    <row r="24" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="27"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+    </row>
+    <row r="25" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="27"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+    </row>
+    <row r="26" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="27"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+    </row>
+    <row r="27" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="27"/>
+      <c r="B27" s="22"/>
+      <c r="C27" s="22"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="27" type="noConversion"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.59055118110236227" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageSetup paperSize="9" scale="64" orientation="landscape" horizontalDpi="4294967294" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Auto-committed on 2022/11/30 週三 11:23:24.66
</commit_message>
<xml_diff>
--- a/Program/Other/LM029_底稿_放款餘額明細表.xlsx
+++ b/Program/Other/LM029_底稿_放款餘額明細表.xlsx
@@ -5,21 +5,18 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\weblogic\itxDoc\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6040" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6040"/>
   </bookViews>
   <sheets>
     <sheet name="la$w30p" sheetId="1" r:id="rId1"/>
     <sheet name="Deliquency" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'la$w30p'!$A$5:$U$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'la$w30p'!$A$5:$W$5</definedName>
     <definedName name="_xlnm.Database" localSheetId="1">#REF!</definedName>
     <definedName name="_xlnm.Database">'la$w30p'!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">Deliquency!#REF!</definedName>
@@ -29,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>戶號</t>
   </si>
@@ -150,6 +147,13 @@
   </si>
   <si>
     <t>放款逾放比</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>企金別</t>
+  </si>
+  <si>
+    <t>行業別</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -163,8 +167,8 @@
     <numFmt numFmtId="177" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="yyyy/mm/dd"/>
-    <numFmt numFmtId="181" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
-    <numFmt numFmtId="192" formatCode="#,##0;[Red]#,##0"/>
+    <numFmt numFmtId="180" formatCode="#,##0.00_);[Red]\(#,##0.00\)"/>
+    <numFmt numFmtId="181" formatCode="#,##0;[Red]#,##0"/>
   </numFmts>
   <fonts count="38" x14ac:knownFonts="1">
     <font>
@@ -632,7 +636,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -771,6 +775,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -925,7 +966,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -981,49 +1022,64 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="24" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="37" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="31" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="181" fontId="35" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="181" fontId="36" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="35" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="24" fillId="0" borderId="10" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" xfId="48" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="37" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="31" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="48" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="192" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="192" fontId="35" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="192" fontId="36" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="34" fillId="0" borderId="10" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="35" fillId="0" borderId="0" xfId="48" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="12" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="13" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="24" fillId="0" borderId="14" xfId="47" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="51">
@@ -1090,19 +1146,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Deliquency "/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1392,13 +1435,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane xSplit="6" ySplit="5" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -1415,11 +1458,13 @@
     <col min="13" max="14" width="17.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="17" width="20.81640625" style="2" customWidth="1"/>
     <col min="18" max="18" width="12.453125" style="1" customWidth="1"/>
-    <col min="19" max="20" width="22.36328125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="22.36328125" customWidth="1"/>
+    <col min="22" max="22" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A1" s="6"/>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -1439,97 +1484,105 @@
       <c r="Q1" s="8"/>
       <c r="R1" s="9"/>
       <c r="S1" s="10"/>
-      <c r="T1" s="18" t="s">
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="18"/>
-    </row>
-    <row r="2" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="W1" s="32"/>
+    </row>
+    <row r="2" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="18" t="s">
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
+      <c r="S2" s="36"/>
+      <c r="T2" s="36"/>
+      <c r="U2" s="37"/>
+      <c r="V2" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="18"/>
-    </row>
-    <row r="3" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="W2" s="32"/>
+    </row>
+    <row r="3" spans="1:23" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="19"/>
-      <c r="R3" s="19"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="18" t="s">
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+      <c r="P3" s="36"/>
+      <c r="Q3" s="36"/>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+      <c r="U3" s="37"/>
+      <c r="V3" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="U3" s="18"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.4">
+      <c r="W3" s="32"/>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
       <c r="T4" s="18"/>
       <c r="U4" s="18"/>
-    </row>
-    <row r="5" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="V4" s="32"/>
+      <c r="W4" s="32"/>
+    </row>
+    <row r="5" spans="1:23" s="17" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
@@ -1594,17 +1647,23 @@
       <c r="U5" s="17" t="s">
         <v>25</v>
       </c>
+      <c r="V5" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="17" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:U5"/>
+  <autoFilter ref="A5:W5"/>
   <mergeCells count="7">
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="T4:U4"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="T2:U2"/>
-    <mergeCell ref="C2:S2"/>
-    <mergeCell ref="C3:S3"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="V4:W4"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="V2:W2"/>
     <mergeCell ref="C4:S4"/>
+    <mergeCell ref="C2:U2"/>
+    <mergeCell ref="C3:U3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1617,9 +1676,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BC27"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection activeCell="A13" sqref="A13:XFD15"/>
       <selection pane="topRight" activeCell="A13" sqref="A13:XFD15"/>
@@ -1629,179 +1688,179 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="27.1796875" style="27" customWidth="1"/>
-    <col min="2" max="2" width="12" style="22" customWidth="1"/>
-    <col min="3" max="16384" width="8.90625" style="22"/>
+    <col min="1" max="1" width="27.1796875" style="26" customWidth="1"/>
+    <col min="2" max="2" width="12" style="21" customWidth="1"/>
+    <col min="3" max="16384" width="8.90625" style="21"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="24" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:5" s="23" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="29" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="28" t="s">
+    <row r="3" spans="1:5" s="28" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="27" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="29" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:5" s="28" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="30"/>
-    </row>
-    <row r="5" spans="1:5" s="32" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="31" t="s">
+      <c r="B4" s="29"/>
+    </row>
+    <row r="5" spans="1:5" s="31" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="29" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:5" s="28" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="27" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="32" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="31" t="s">
+    <row r="7" spans="1:5" s="31" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="30" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.4">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="B9" s="26"/>
-    </row>
-    <row r="10" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="27"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-    </row>
-    <row r="11" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="27"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="27"/>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-    </row>
-    <row r="13" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="27"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-    </row>
-    <row r="14" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="27"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-    </row>
-    <row r="15" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="27"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-    </row>
-    <row r="16" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="27"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-    </row>
-    <row r="17" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="27"/>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-    </row>
-    <row r="18" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="27"/>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-    </row>
-    <row r="19" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="27"/>
-      <c r="B19" s="22"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="22"/>
-      <c r="E19" s="22"/>
-    </row>
-    <row r="20" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="27"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-    </row>
-    <row r="21" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="27"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-    </row>
-    <row r="22" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="27"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-    </row>
-    <row r="23" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="27"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
-    </row>
-    <row r="24" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="27"/>
-      <c r="B24" s="22"/>
-      <c r="C24" s="22"/>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
-    </row>
-    <row r="25" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="27"/>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-    </row>
-    <row r="26" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="27"/>
-      <c r="B26" s="22"/>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-    </row>
-    <row r="27" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="27"/>
-      <c r="B27" s="22"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
+      <c r="B9" s="25"/>
+    </row>
+    <row r="10" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="26"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+    </row>
+    <row r="11" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="26"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+    </row>
+    <row r="12" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="26"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+    </row>
+    <row r="13" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="26"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+    </row>
+    <row r="14" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="26"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+    </row>
+    <row r="15" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="26"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+    </row>
+    <row r="16" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="26"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+    </row>
+    <row r="17" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A17" s="26"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+    </row>
+    <row r="18" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="26"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+    </row>
+    <row r="19" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="26"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+    </row>
+    <row r="20" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="26"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+    </row>
+    <row r="21" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="26"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+    </row>
+    <row r="22" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A22" s="26"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+    </row>
+    <row r="23" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="26"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+    </row>
+    <row r="24" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A24" s="26"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+    </row>
+    <row r="25" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A25" s="26"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+    </row>
+    <row r="26" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="26"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+    </row>
+    <row r="27" spans="1:5" s="20" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A27" s="26"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="27" type="noConversion"/>

</xml_diff>